<commit_message>
added calculation of % abundance
</commit_message>
<xml_diff>
--- a/data/Mass Spec and Protein Properties 200CMNP.xlsx
+++ b/data/Mass Spec and Protein Properties 200CMNP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavo/PycharmProjects/swnt-protein-corona-ML/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE03DB0-6E34-7347-8EA3-ED400605A8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340340EF-5F56-4945-8A43-5A3B1F9D0D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="760" windowWidth="19780" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protein Properties" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="821">
   <si>
     <t>Entry</t>
   </si>
@@ -2475,6 +2475,15 @@
   </si>
   <si>
     <t>Accession</t>
+  </si>
+  <si>
+    <t>Relative Abundance_1</t>
+  </si>
+  <si>
+    <t>Relative Abundance_2</t>
+  </si>
+  <si>
+    <t>Relative Abundance_3</t>
   </si>
 </sst>
 </file>
@@ -6312,1032 +6321,2871 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67499FF8-0E27-8146-BF0C-A25E26B61179}">
-  <dimension ref="A1:A204"/>
+  <dimension ref="A1:D204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C1" t="s">
+        <v>819</v>
+      </c>
+      <c r="D1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1066.7724501860801</v>
+      </c>
+      <c r="C2">
+        <v>1429.0468214180701</v>
+      </c>
+      <c r="D2">
+        <v>1385.3965053289501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1525.9871155140299</v>
+      </c>
+      <c r="C3">
+        <v>1563.6581708578999</v>
+      </c>
+      <c r="D3">
+        <v>738.34407099021803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1329.03564004847</v>
+      </c>
+      <c r="C4">
+        <v>1491.24158313213</v>
+      </c>
+      <c r="D4">
+        <v>682.86473093507595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1276.1812852897001</v>
+      </c>
+      <c r="C5">
+        <v>1260.7984162017201</v>
+      </c>
+      <c r="D5">
+        <v>750.86842591587595</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1164.7524525872</v>
+      </c>
+      <c r="C6">
+        <v>528.87695627897301</v>
+      </c>
+      <c r="D6">
+        <v>1133.39567822666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>928.75119499363905</v>
+      </c>
+      <c r="C7">
+        <v>824.06502694443805</v>
+      </c>
+      <c r="D7">
+        <v>934.93984133782203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>723.71513991677705</v>
+      </c>
+      <c r="C8">
+        <v>784.06311019401903</v>
+      </c>
+      <c r="D8">
+        <v>893.49775942747704</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>800.06026839285403</v>
+      </c>
+      <c r="C9">
+        <v>709.53896618720501</v>
+      </c>
+      <c r="D9">
+        <v>734.02871915415005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>715.88483862250496</v>
+      </c>
+      <c r="C10">
+        <v>520.15154810185902</v>
+      </c>
+      <c r="D10">
+        <v>917.80249345429797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>655.45452596924804</v>
+      </c>
+      <c r="C11">
+        <v>597.62628169296397</v>
+      </c>
+      <c r="D11">
+        <v>699.48127034545405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>603.94764453419998</v>
+      </c>
+      <c r="C12">
+        <v>638.80849902205603</v>
+      </c>
+      <c r="D12">
+        <v>694.57069975578997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>429.16481919463001</v>
+      </c>
+      <c r="C13">
+        <v>863.603315843671</v>
+      </c>
+      <c r="D13">
+        <v>502.53824144075298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>507.289537934767</v>
+      </c>
+      <c r="C14">
+        <v>520.88920898646495</v>
+      </c>
+      <c r="D14">
+        <v>628.10460560427896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>394.81840493862899</v>
+      </c>
+      <c r="C15">
+        <v>391.48359693843298</v>
+      </c>
+      <c r="D15">
+        <v>419.75321725566198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>383.35267867077903</v>
+      </c>
+      <c r="C16">
+        <v>392.55844416727098</v>
+      </c>
+      <c r="D16">
+        <v>429.74794009603801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>369.64970021786701</v>
+      </c>
+      <c r="C17">
+        <v>365.41277180279798</v>
+      </c>
+      <c r="D17">
+        <v>410.94893192247599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>335.40497776385303</v>
+      </c>
+      <c r="C18">
+        <v>286.504854619112</v>
+      </c>
+      <c r="D18">
+        <v>430.83917447763002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>290.60975525985799</v>
+      </c>
+      <c r="C19">
+        <v>310.53130376157998</v>
+      </c>
+      <c r="D19">
+        <v>372.80534600205698</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>326.55779099109998</v>
+      </c>
+      <c r="C20">
+        <v>295.94682761544999</v>
+      </c>
+      <c r="D20">
+        <v>336.74499397422198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>272.66113593870102</v>
+      </c>
+      <c r="C21">
+        <v>290.909723861364</v>
+      </c>
+      <c r="D21">
+        <v>364.69548254806699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>262.61907862796198</v>
+      </c>
+      <c r="C22">
+        <v>286.73669552177</v>
+      </c>
+      <c r="D22">
+        <v>304.03278711661301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>255.14473118201599</v>
+      </c>
+      <c r="C23">
+        <v>259.696395575937</v>
+      </c>
+      <c r="D23">
+        <v>270.00611503606302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>244.17981670058401</v>
+      </c>
+      <c r="C24">
+        <v>215.078864745987</v>
+      </c>
+      <c r="D24">
+        <v>289.127493686572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>204.509844745979</v>
+      </c>
+      <c r="C25">
+        <v>213.79324570280599</v>
+      </c>
+      <c r="D25">
+        <v>240.28236662400701</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>189.58148821448501</v>
+      </c>
+      <c r="C26">
+        <v>251.835116767448</v>
+      </c>
+      <c r="D26">
+        <v>213.636407088043</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>187.21714568297401</v>
+      </c>
+      <c r="C27">
+        <v>214.40443810339201</v>
+      </c>
+      <c r="D27">
+        <v>218.58664305544599</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>177.42168692437701</v>
+      </c>
+      <c r="C28">
+        <v>182.49774527524499</v>
+      </c>
+      <c r="D28">
+        <v>228.24655137880001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>175.959863203162</v>
+      </c>
+      <c r="C29">
+        <v>195.95466100615201</v>
+      </c>
+      <c r="D29">
+        <v>199.76533401924999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>175.743772191614</v>
+      </c>
+      <c r="C30">
+        <v>179.214123814841</v>
+      </c>
+      <c r="D30">
+        <v>183.75642565754299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>140.84314575013599</v>
+      </c>
+      <c r="C31">
+        <v>170.674196452975</v>
+      </c>
+      <c r="D31">
+        <v>177.95304280998499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>150.94114168731201</v>
+      </c>
+      <c r="C32">
+        <v>143.20184531136101</v>
+      </c>
+      <c r="D32">
+        <v>183.90275423592701</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>116.627789469973</v>
+      </c>
+      <c r="C33">
+        <v>141.54108319250199</v>
+      </c>
+      <c r="D33">
+        <v>154.749431732316</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>135.23738923334901</v>
+      </c>
+      <c r="C34">
+        <v>129.285483174452</v>
+      </c>
+      <c r="D34">
+        <v>148.199549332749</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>124.74533349580599</v>
+      </c>
+      <c r="C35">
+        <v>120.448389945325</v>
+      </c>
+      <c r="D35">
+        <v>132.08400157914801</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>119.63277408330499</v>
+      </c>
+      <c r="C36">
+        <v>125.179910987651</v>
+      </c>
+      <c r="D36">
+        <v>124.601601862698</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>101.81891673814</v>
+      </c>
+      <c r="C37">
+        <v>121.407330211366</v>
+      </c>
+      <c r="D37">
+        <v>135.662750367016</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>99.096122807646296</v>
+      </c>
+      <c r="C38">
+        <v>113.34582762122299</v>
+      </c>
+      <c r="D38">
+        <v>107.727150198262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>105.111184759753</v>
+      </c>
+      <c r="C39">
+        <v>94.737978407492506</v>
+      </c>
+      <c r="D39">
+        <v>116.732317892661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>116.762527039932</v>
+      </c>
+      <c r="C40">
+        <v>95.614733042866803</v>
+      </c>
+      <c r="D40">
+        <v>100.26212293316701</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>92.882753706322603</v>
+      </c>
+      <c r="C41">
+        <v>102.67092179102301</v>
+      </c>
+      <c r="D41">
+        <v>108.49349831164101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>102.357883288664</v>
+      </c>
+      <c r="C42">
+        <v>91.4901892346099</v>
+      </c>
+      <c r="D42">
+        <v>109.542567396729</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>132.88576224475801</v>
+      </c>
+      <c r="C43">
+        <v>160.94559213353301</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>87.210889382900405</v>
+      </c>
+      <c r="C44">
+        <v>87.418338379938902</v>
+      </c>
+      <c r="D44">
+        <v>114.81769756859499</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>88.304076254246297</v>
+      </c>
+      <c r="C45">
+        <v>94.293274967897901</v>
+      </c>
+      <c r="D45">
+        <v>105.274356885945</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>90.315027570840599</v>
+      </c>
+      <c r="C46">
+        <v>92.716802690830605</v>
+      </c>
+      <c r="D46">
+        <v>98.057329498598605</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>77.217123475087803</v>
+      </c>
+      <c r="C47">
+        <v>89.715604131280202</v>
+      </c>
+      <c r="D47">
+        <v>83.107418470788602</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>74.0697703389759</v>
+      </c>
+      <c r="C48">
+        <v>79.1882223848812</v>
+      </c>
+      <c r="D48">
+        <v>90.341810373240406</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>71.631705318697598</v>
+      </c>
+      <c r="C49">
+        <v>69.086579200887201</v>
+      </c>
+      <c r="D49">
+        <v>71.9495508871357</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>71.334260865561603</v>
+      </c>
+      <c r="C50">
+        <v>52.5884174563922</v>
+      </c>
+      <c r="D50">
+        <v>82.909012219589997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>57.234688452578098</v>
+      </c>
+      <c r="C51">
+        <v>56.114404247212299</v>
+      </c>
+      <c r="D51">
+        <v>78.549034849502107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>79.100968174544207</v>
+      </c>
+      <c r="C52">
+        <v>35.276728574266301</v>
+      </c>
+      <c r="D52">
+        <v>75.828393098067195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>63.745506074709802</v>
+      </c>
+      <c r="C53">
+        <v>64.481513154047306</v>
+      </c>
+      <c r="D53">
+        <v>57.937105428113703</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>56.998255012961401</v>
+      </c>
+      <c r="C54">
+        <v>61.499279471686599</v>
+      </c>
+      <c r="D54">
+        <v>64.008336714789095</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>50.446760670035403</v>
+      </c>
+      <c r="C55">
+        <v>68.968554538432898</v>
+      </c>
+      <c r="D55">
+        <v>53.145594461668999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>62.515035270683299</v>
+      </c>
+      <c r="C56">
+        <v>45.213983636260899</v>
+      </c>
+      <c r="D56">
+        <v>61.887869905104701</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>64.131934922255297</v>
+      </c>
+      <c r="C57">
+        <v>41.721718177570501</v>
+      </c>
+      <c r="D57">
+        <v>62.964223817856798</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>53.2763350602863</v>
+      </c>
+      <c r="C58">
+        <v>50.139405710466903</v>
+      </c>
+      <c r="D58">
+        <v>59.8542058303196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>67.345395865002104</v>
+      </c>
+      <c r="C59">
+        <v>29.765398354305301</v>
+      </c>
+      <c r="D59">
+        <v>63.529681633772597</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>57.766028117953098</v>
+      </c>
+      <c r="C60">
+        <v>43.981047430265797</v>
+      </c>
+      <c r="D60">
+        <v>57.396448393597701</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>55.076279955432497</v>
+      </c>
+      <c r="C61">
+        <v>36.180881791996001</v>
+      </c>
+      <c r="D61">
+        <v>53.440723760326797</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>42.931736503295198</v>
+      </c>
+      <c r="C62">
+        <v>44.027414261944202</v>
+      </c>
+      <c r="D62">
+        <v>53.406002666367101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>39.069990322889801</v>
+      </c>
+      <c r="C63">
+        <v>42.823984221562696</v>
+      </c>
+      <c r="D63">
+        <v>51.362418279022101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>42.329212576530203</v>
+      </c>
+      <c r="C64">
+        <v>38.484470293111599</v>
+      </c>
+      <c r="D64">
+        <v>46.697391297716401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>33.512533344373601</v>
+      </c>
+      <c r="C65">
+        <v>47.542863136473798</v>
+      </c>
+      <c r="D65">
+        <v>42.275411974129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>41.523305045793897</v>
+      </c>
+      <c r="C66">
+        <v>36.733068605621199</v>
+      </c>
+      <c r="D66">
+        <v>41.3106615776761</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>32.805775320573296</v>
+      </c>
+      <c r="C67">
+        <v>41.131594865299398</v>
+      </c>
+      <c r="D67">
+        <v>42.449017443927701</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>36.581083469290903</v>
+      </c>
+      <c r="C68">
+        <v>34.813060257481801</v>
+      </c>
+      <c r="D68">
+        <v>40.422793603562603</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>33.886250716670901</v>
+      </c>
+      <c r="C69">
+        <v>35.653985977468203</v>
+      </c>
+      <c r="D69">
+        <v>40.040861570005397</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>36.743790352467897</v>
+      </c>
+      <c r="C70">
+        <v>32.2291631830374</v>
+      </c>
+      <c r="D70">
+        <v>36.506750220531401</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>31.646488777936799</v>
+      </c>
+      <c r="C71">
+        <v>32.361940928298402</v>
+      </c>
+      <c r="D71">
+        <v>36.821720144309097</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>29.788071096648899</v>
+      </c>
+      <c r="C72">
+        <v>31.3608388806955</v>
+      </c>
+      <c r="D72">
+        <v>36.246342015833299</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>32.017663855184402</v>
+      </c>
+      <c r="C73">
+        <v>29.253255622584302</v>
+      </c>
+      <c r="D73">
+        <v>32.057490037404101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>30.451610104605301</v>
+      </c>
+      <c r="C74">
+        <v>26.576624884783001</v>
+      </c>
+      <c r="D74">
+        <v>35.266711150540502</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>27.1059498192772</v>
+      </c>
+      <c r="C75">
+        <v>26.020222904641599</v>
+      </c>
+      <c r="D75">
+        <v>36.784518972209398</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>27.843215383673201</v>
+      </c>
+      <c r="C76">
+        <v>26.488106387942299</v>
+      </c>
+      <c r="D76">
+        <v>33.629859578152598</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>28.880471763926899</v>
+      </c>
+      <c r="C77">
+        <v>28.524031815277802</v>
+      </c>
+      <c r="D77">
+        <v>30.442959168276001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>27.243233751957799</v>
+      </c>
+      <c r="C78">
+        <v>25.147683435783499</v>
+      </c>
+      <c r="D78">
+        <v>28.0695243883135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>26.096658684569501</v>
+      </c>
+      <c r="C79">
+        <v>25.531263588759799</v>
+      </c>
+      <c r="D79">
+        <v>25.3141575747937</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>29.950777979825901</v>
+      </c>
+      <c r="C80">
+        <v>13.8609428136203</v>
+      </c>
+      <c r="D80">
+        <v>27.962881028294198</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>20.004302827608701</v>
+      </c>
+      <c r="C81">
+        <v>24.795717031679001</v>
+      </c>
+      <c r="D81">
+        <v>20.902098563766199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>22.2661827332747</v>
+      </c>
+      <c r="C82">
+        <v>20.4077286882913</v>
+      </c>
+      <c r="D82">
+        <v>20.861425282270499</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>20.6864005894275</v>
+      </c>
+      <c r="C83">
+        <v>19.5318170862203</v>
+      </c>
+      <c r="D83">
+        <v>22.884425021053602</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>18.306812422963102</v>
+      </c>
+      <c r="C84">
+        <v>17.980846566576201</v>
+      </c>
+      <c r="D84">
+        <v>26.566597035484499</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>16.134675532549402</v>
+      </c>
+      <c r="C85">
+        <v>20.4121546131333</v>
+      </c>
+      <c r="D85">
+        <v>24.1011513565287</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>18.3312184554397</v>
+      </c>
+      <c r="C86">
+        <v>17.420440178244402</v>
+      </c>
+      <c r="D86">
+        <v>21.6939875138624</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>17.649120693620901</v>
+      </c>
+      <c r="C87">
+        <v>19.068148769435801</v>
+      </c>
+      <c r="D87">
+        <v>20.401866802931899</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>18.166477736222902</v>
+      </c>
+      <c r="C88">
+        <v>17.7167663843349</v>
+      </c>
+      <c r="D88">
+        <v>21.021638330113301</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>18.4085042249488</v>
+      </c>
+      <c r="C89">
+        <v>16.258951044699302</v>
+      </c>
+      <c r="D89">
+        <v>19.5933613292978</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>18.263084948109299</v>
+      </c>
+      <c r="C90">
+        <v>17.1652118456871</v>
+      </c>
+      <c r="D90">
+        <v>18.6541557376867</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>23.832236483853801</v>
+      </c>
+      <c r="C91">
+        <v>9.2438601700759992</v>
+      </c>
+      <c r="D91">
+        <v>20.2237971924812</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>15.657995210741699</v>
+      </c>
+      <c r="C92">
+        <v>16.405217322812199</v>
+      </c>
+      <c r="D92">
+        <v>20.304151724216599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>13.815085529256599</v>
+      </c>
+      <c r="C93">
+        <v>18.895537700596499</v>
+      </c>
+      <c r="D93">
+        <v>17.940389248999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>19.5947390951115</v>
+      </c>
+      <c r="C94">
+        <v>9.7671730930650202</v>
+      </c>
+      <c r="D94">
+        <v>20.099545277668099</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>17.388281221527699</v>
+      </c>
+      <c r="C95">
+        <v>15.731422955194001</v>
+      </c>
+      <c r="D95">
+        <v>16.337514747129799</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>15.3635974439932</v>
+      </c>
+      <c r="C96">
+        <v>16.2966767850195</v>
+      </c>
+      <c r="D96">
+        <v>17.4649582695655</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>14.5050644057293</v>
+      </c>
+      <c r="C97">
+        <v>16.602065599119801</v>
+      </c>
+      <c r="D97">
+        <v>17.657164325414101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>15.1233505618021</v>
+      </c>
+      <c r="C98">
+        <v>15.834905293167299</v>
+      </c>
+      <c r="D98">
+        <v>16.875195687877799</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>16.749656705057699</v>
+      </c>
+      <c r="C99">
+        <v>15.021167397210499</v>
+      </c>
+      <c r="D99">
+        <v>16.022544823352099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>17.662340627879001</v>
+      </c>
+      <c r="C100">
+        <v>13.2885232007173</v>
+      </c>
+      <c r="D100">
+        <v>16.258152246650301</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>13.6376333347916</v>
+      </c>
+      <c r="C101">
+        <v>14.5282036731383</v>
+      </c>
+      <c r="D101">
+        <v>14.3008745785767</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>13.617549203899401</v>
+      </c>
+      <c r="C102">
+        <v>13.495277118338</v>
+      </c>
+      <c r="D102">
+        <v>15.2591767718657</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>12.5462260699805</v>
+      </c>
+      <c r="C103">
+        <v>12.263394703972001</v>
+      </c>
+      <c r="D103">
+        <v>14.7465446203315</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>13.7225459894496</v>
+      </c>
+      <c r="C104">
+        <v>9.6468300890268708</v>
+      </c>
+      <c r="D104">
+        <v>13.253785587876401</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>8.0639056679577301</v>
+      </c>
+      <c r="C105">
+        <v>20.273686393075401</v>
+      </c>
+      <c r="D105">
+        <v>7.1587455510573301</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>10.129520395791401</v>
+      </c>
+      <c r="C106">
+        <v>11.065022863409901</v>
+      </c>
+      <c r="D106">
+        <v>13.6062046915679</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>11.3137214299144</v>
+      </c>
+      <c r="C107">
+        <v>12.066335669338599</v>
+      </c>
+      <c r="D107">
+        <v>10.221642053934801</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>10.8011947479066</v>
+      </c>
+      <c r="C108">
+        <v>11.618895743641501</v>
+      </c>
+      <c r="D108">
+        <v>10.466673774165001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>12.6090207577067</v>
+      </c>
+      <c r="C109">
+        <v>7.8250351207154898</v>
+      </c>
+      <c r="D109">
+        <v>11.8743661264186</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>12.3497066626432</v>
+      </c>
+      <c r="C110">
+        <v>11.394016610001101</v>
+      </c>
+      <c r="D110">
+        <v>7.9942838764171897</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>10.7017910114657</v>
+      </c>
+      <c r="C111">
+        <v>10.025984317161001</v>
+      </c>
+      <c r="D111">
+        <v>10.740970416446901</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>9.6007230254659905</v>
+      </c>
+      <c r="C112">
+        <v>10.596507105131799</v>
+      </c>
+      <c r="D112">
+        <v>10.5336358839445</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>9.5928419108120995</v>
+      </c>
+      <c r="C113">
+        <v>8.2830129627030704</v>
+      </c>
+      <c r="D113">
+        <v>11.5936212809727</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>10.0245236102412</v>
+      </c>
+      <c r="C114">
+        <v>8.3481372853787104</v>
+      </c>
+      <c r="D114">
+        <v>11.0685887387385</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>10.0758779702439</v>
+      </c>
+      <c r="C115">
+        <v>8.71232767238034</v>
+      </c>
+      <c r="D115">
+        <v>10.327045374883999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>10.1236731171772</v>
+      </c>
+      <c r="C116">
+        <v>8.7523717542844501</v>
+      </c>
+      <c r="D116">
+        <v>9.7576194339442193</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>10.8042455019662</v>
+      </c>
+      <c r="C117">
+        <v>8.5894555684324505</v>
+      </c>
+      <c r="D117">
+        <v>8.9568022025441092</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>9.0686206715760296</v>
+      </c>
+      <c r="C118">
+        <v>9.6529420804753894</v>
+      </c>
+      <c r="D118">
+        <v>8.2980934485649502</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>8.3399989103487897</v>
+      </c>
+      <c r="C119">
+        <v>8.3765896593632103</v>
+      </c>
+      <c r="D119">
+        <v>9.7968046685559198</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>12.0441227976763</v>
+      </c>
+      <c r="C120">
+        <v>4.2413005486230997</v>
+      </c>
+      <c r="D120">
+        <v>9.7625795902241794</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>7.97060343963589</v>
+      </c>
+      <c r="C121">
+        <v>8.2404397808892202</v>
+      </c>
+      <c r="D121">
+        <v>9.3856077129469497</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>8.3593203527260602</v>
+      </c>
+      <c r="C122">
+        <v>8.5125287795113902</v>
+      </c>
+      <c r="D122">
+        <v>8.6750653258421799</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>7.2480831865277899</v>
+      </c>
+      <c r="C123">
+        <v>8.2100905819724197</v>
+      </c>
+      <c r="D123">
+        <v>9.93072888811494</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>7.2351174817746102</v>
+      </c>
+      <c r="C124">
+        <v>7.7712917476336596</v>
+      </c>
+      <c r="D124">
+        <v>9.4902670104541809</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>8.1856816008355597</v>
+      </c>
+      <c r="C125">
+        <v>8.3671055347017091</v>
+      </c>
+      <c r="D125">
+        <v>7.9245936806837003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>6.9605496164133402</v>
+      </c>
+      <c r="C126">
+        <v>7.8570703862387798</v>
+      </c>
+      <c r="D126">
+        <v>9.5986464251713794</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>8.2355105838085301</v>
+      </c>
+      <c r="C127">
+        <v>6.8184533566415499</v>
+      </c>
+      <c r="D127">
+        <v>8.9734187260819809</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>7.7382376720986601</v>
+      </c>
+      <c r="C128">
+        <v>6.4875627851180804</v>
+      </c>
+      <c r="D128">
+        <v>9.1438000942987294</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>6.5713242443132298</v>
+      </c>
+      <c r="C129">
+        <v>8.2124089235563407</v>
+      </c>
+      <c r="D129">
+        <v>7.9231056337997101</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>7.6884086891256898</v>
+      </c>
+      <c r="C130">
+        <v>7.2814893984486</v>
+      </c>
+      <c r="D130">
+        <v>7.5627502800603601</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>7.6873917711058297</v>
+      </c>
+      <c r="C131">
+        <v>6.50800634272177</v>
+      </c>
+      <c r="D131">
+        <v>8.3290944253147199</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>6.4137019512354598</v>
+      </c>
+      <c r="C132">
+        <v>7.1670476275331598</v>
+      </c>
+      <c r="D132">
+        <v>8.7073063416619405</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>6.6076790635230997</v>
+      </c>
+      <c r="C133">
+        <v>6.1058794570741401</v>
+      </c>
+      <c r="D133">
+        <v>9.27450021227577</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B134">
+        <v>7.0426657465167599</v>
+      </c>
+      <c r="C134">
+        <v>7.88130759370706</v>
+      </c>
+      <c r="D134">
+        <v>6.9675315264647404</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>7.2732519075192403</v>
+      </c>
+      <c r="C135">
+        <v>6.4215954291391997</v>
+      </c>
+      <c r="D135">
+        <v>7.8586236021601801</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <v>5.2358566547365699</v>
+      </c>
+      <c r="C136">
+        <v>8.1278948349060798</v>
+      </c>
+      <c r="D136">
+        <v>8.1773136431478406</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>5.8932941545738498</v>
+      </c>
+      <c r="C137">
+        <v>7.5628517634064503</v>
+      </c>
+      <c r="D137">
+        <v>6.8842009009613498</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>6.0877797258714299</v>
+      </c>
+      <c r="C138">
+        <v>6.5569022743099499</v>
+      </c>
+      <c r="D138">
+        <v>7.1096400038856897</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>6.6229328338209497</v>
+      </c>
+      <c r="C139">
+        <v>6.2333882441898698</v>
+      </c>
+      <c r="D139">
+        <v>6.5724550787656497</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>5.2048406551309503</v>
+      </c>
+      <c r="C140">
+        <v>5.7062816713362396</v>
+      </c>
+      <c r="D140">
+        <v>7.5999514521600897</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>6.1998949375606101</v>
+      </c>
+      <c r="C141">
+        <v>6.11135917354523</v>
+      </c>
+      <c r="D141">
+        <v>6.0565988256494396</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B142">
+        <v>5.6759279278295098</v>
+      </c>
+      <c r="C142">
+        <v>5.9393803796833504</v>
+      </c>
+      <c r="D142">
+        <v>6.5305417581999503</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B143">
+        <v>8.5349929406562897</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>8.9833390386419101</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B144">
+        <v>6.0015959236885799</v>
+      </c>
+      <c r="C144">
+        <v>5.5117517366125703</v>
+      </c>
+      <c r="D144">
+        <v>5.8527364025429396</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>7.3794920199507699</v>
+      </c>
+      <c r="D145">
+        <v>9.9684260758426593</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B146">
+        <v>6.0112566448772196</v>
+      </c>
+      <c r="C146">
+        <v>4.7397439891664197</v>
+      </c>
+      <c r="D146">
+        <v>6.1835788264165101</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>4.7429056446111</v>
+      </c>
+      <c r="C147">
+        <v>4.9633585728520204</v>
+      </c>
+      <c r="D147">
+        <v>7.1934666450170797</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>6.8369940770007602</v>
+      </c>
+      <c r="C148">
+        <v>3.7093465342758201</v>
+      </c>
+      <c r="D148">
+        <v>6.0332860911336104</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B149">
+        <v>6.3468395914298901</v>
+      </c>
+      <c r="C149">
+        <v>5.0238462123598104</v>
+      </c>
+      <c r="D149">
+        <v>4.9626363581034898</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>6.4398875902467703</v>
+      </c>
+      <c r="C150">
+        <v>5.8453821663715804</v>
+      </c>
+      <c r="D150">
+        <v>3.9351399847090498</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>8.8141239437471093</v>
+      </c>
+      <c r="D151">
+        <v>7.3539277006738999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B152">
+        <v>4.3707136493435899</v>
+      </c>
+      <c r="C152">
+        <v>7.1274250622806603</v>
+      </c>
+      <c r="D152">
+        <v>4.5387910039806103</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B153">
+        <v>4.5237598113319999</v>
+      </c>
+      <c r="C153">
+        <v>4.96167250624553</v>
+      </c>
+      <c r="D153">
+        <v>6.4159621481327997</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B154">
+        <v>5.22619593354794</v>
+      </c>
+      <c r="C154">
+        <v>3.37044714637153</v>
+      </c>
+      <c r="D154">
+        <v>7.1322087149595301</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B155">
+        <v>4.8242590861996204</v>
+      </c>
+      <c r="C155">
+        <v>5.8354765250584597</v>
+      </c>
+      <c r="D155">
+        <v>4.7009881143354102</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B156">
+        <v>4.8308690533286898</v>
+      </c>
+      <c r="C156">
+        <v>4.4261356003594603</v>
+      </c>
+      <c r="D156">
+        <v>6.0526307006254703</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B157">
+        <v>4.3038512895380201</v>
+      </c>
+      <c r="C157">
+        <v>5.4481027222176097</v>
+      </c>
+      <c r="D157">
+        <v>5.1903075313538096</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B158">
+        <v>7.05308915622029</v>
+      </c>
+      <c r="C158">
+        <v>3.1698052201993399</v>
+      </c>
+      <c r="D158">
+        <v>4.6875956923795101</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B159">
+        <v>5.6756736983245499</v>
+      </c>
+      <c r="C159">
+        <v>5.2535727874939404</v>
+      </c>
+      <c r="D159">
+        <v>3.59313720920556</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B160">
+        <v>5.0177277394773396</v>
+      </c>
+      <c r="C160">
+        <v>4.4779821485089997</v>
+      </c>
+      <c r="D160">
+        <v>4.7934950289567304</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B161">
+        <v>4.0407237519001296</v>
+      </c>
+      <c r="C161">
+        <v>4.9079291331636901</v>
+      </c>
+      <c r="D161">
+        <v>5.3150554617948904</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B162">
+        <v>4.5247767293518599</v>
+      </c>
+      <c r="C162">
+        <v>4.8615623014852503</v>
+      </c>
+      <c r="D162">
+        <v>4.75182971620504</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B163">
+        <v>4.7904465620393903</v>
+      </c>
+      <c r="C163">
+        <v>4.5679759536303504</v>
+      </c>
+      <c r="D163">
+        <v>4.4807571755050297</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B164">
+        <v>5.0657771159155596</v>
+      </c>
+      <c r="C164">
+        <v>3.59258642177645</v>
+      </c>
+      <c r="D164">
+        <v>5.0452229601648799</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B165">
+        <v>4.4223222388513097</v>
+      </c>
+      <c r="C165">
+        <v>3.5725643808243999</v>
+      </c>
+      <c r="D165">
+        <v>5.0221582334630499</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B166">
+        <v>3.7414956245573299</v>
+      </c>
+      <c r="C166">
+        <v>4.9384890904063097</v>
+      </c>
+      <c r="D166">
+        <v>4.2203489708069499</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B167">
+        <v>5.5211021593063396</v>
+      </c>
+      <c r="C167">
+        <v>3.4172354947015999</v>
+      </c>
+      <c r="D167">
+        <v>3.8294886559458199</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B168">
+        <v>4.4279152879605199</v>
+      </c>
+      <c r="C168">
+        <v>3.5346278821783899</v>
+      </c>
+      <c r="D168">
+        <v>4.6454343639998203</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B169">
+        <v>4.92061206858103</v>
+      </c>
+      <c r="C169">
+        <v>4.5171831971098699</v>
+      </c>
+      <c r="D169">
+        <v>3.0291674401737101</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B170">
+        <v>3.08354966571012</v>
+      </c>
+      <c r="C170">
+        <v>3.9808032579205501</v>
+      </c>
+      <c r="D170">
+        <v>5.34630444635867</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B171">
+        <v>3.31083084314806</v>
+      </c>
+      <c r="C171">
+        <v>3.3548510302615</v>
+      </c>
+      <c r="D171">
+        <v>5.2056840158217002</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B172">
+        <v>3.7209030346552301</v>
+      </c>
+      <c r="C172">
+        <v>3.5820485054859001</v>
+      </c>
+      <c r="D172">
+        <v>4.5363109258406196</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B173">
+        <v>2.94779111005926</v>
+      </c>
+      <c r="C173">
+        <v>3.6676163857652102</v>
+      </c>
+      <c r="D173">
+        <v>3.6819240066169101</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B174">
+        <v>3.60090670831215</v>
+      </c>
+      <c r="C174">
+        <v>3.5171349411360699</v>
+      </c>
+      <c r="D174">
+        <v>3.1010897062331799</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B175">
+        <v>3.7720031651530199</v>
+      </c>
+      <c r="C175">
+        <v>3.03386610005116</v>
+      </c>
+      <c r="D175">
+        <v>3.3766263875851599</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176">
+        <v>3.4824357589988599</v>
+      </c>
+      <c r="C176">
+        <v>3.3470529722064901</v>
+      </c>
+      <c r="D176">
+        <v>3.22806970700025</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177">
+        <v>3.6225162162341098</v>
+      </c>
+      <c r="C177">
+        <v>2.0072833708577398</v>
+      </c>
+      <c r="D177">
+        <v>4.3877542452557199</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B178">
+        <v>2.8130494724282702</v>
+      </c>
+      <c r="C178">
+        <v>3.1531553124602598</v>
+      </c>
+      <c r="D178">
+        <v>3.9825094771826999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>5.2297570966772797</v>
+      </c>
+      <c r="D179">
+        <v>4.6360100670678897</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180">
+        <v>3.27676408948287</v>
+      </c>
+      <c r="C180">
+        <v>3.16306095377338</v>
+      </c>
+      <c r="D180">
+        <v>3.3657140437692399</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B181">
+        <v>5.8116864834803597</v>
+      </c>
+      <c r="C181">
+        <v>3.9449743425326602</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B182">
+        <v>3.7915788370352601</v>
+      </c>
+      <c r="C182">
+        <v>1.93543585758873</v>
+      </c>
+      <c r="D182">
+        <v>3.8027038120340202</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B183">
+        <v>3.0301614696676502</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>5.9110182388325097</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>3.4473739352925898</v>
+      </c>
+      <c r="D184">
+        <v>5.3465524541726603</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B185">
+        <v>2.8486416031232502</v>
+      </c>
+      <c r="C185">
+        <v>3.49142242538711</v>
+      </c>
+      <c r="D185">
+        <v>2.3227667835627099</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B186">
+        <v>2.5031437058769699</v>
+      </c>
+      <c r="C186">
+        <v>2.4905311361100702</v>
+      </c>
+      <c r="D186">
+        <v>2.7355261883998701</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B187">
+        <v>1.4964457121199499</v>
+      </c>
+      <c r="C187">
+        <v>2.7128811698408102</v>
+      </c>
+      <c r="D187">
+        <v>3.3734022860031798</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B188">
+        <v>2.07161454415083</v>
+      </c>
+      <c r="C188">
+        <v>2.2780867436924601</v>
+      </c>
+      <c r="D188">
+        <v>2.5353838825033401</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B189">
+        <v>2.9597398967925801</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>3.5274151384960502</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B190">
+        <v>2.40663818579258</v>
+      </c>
+      <c r="C190">
+        <v>2.0282959759411101</v>
+      </c>
+      <c r="D190">
+        <v>1.8841649645069301</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B191">
+        <v>2.9978743225372</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191">
+        <v>3.2766792385438901</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B192">
+        <v>1.59455287808561</v>
+      </c>
+      <c r="C192">
+        <v>1.49166312676082</v>
+      </c>
+      <c r="D192">
+        <v>2.0817775907006801</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B193">
+        <v>2.3609785667010201</v>
+      </c>
+      <c r="C193">
+        <v>1.16985623907981</v>
+      </c>
+      <c r="D193">
+        <v>1.2503561950532001</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>1.72661650837507</v>
+      </c>
+      <c r="D194">
+        <v>2.6636039223404002</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195">
+        <v>4.1595870563773998</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B196">
+        <v>1.5864175339267601</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>1.6771280413812599</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>3.1847690613319202</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B198">
+        <v>0</v>
+      </c>
+      <c r="C198">
+        <v>2.8235292908916501</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B199">
+        <v>0</v>
+      </c>
+      <c r="C199">
+        <v>0</v>
+      </c>
+      <c r="D199">
+        <v>2.6030900157248502</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>2.2730285438729898</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B201">
+        <v>0</v>
+      </c>
+      <c r="C201">
+        <v>0</v>
+      </c>
+      <c r="D201">
+        <v>1.9458693086296801</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B202">
+        <v>0</v>
+      </c>
+      <c r="C202">
+        <v>0</v>
+      </c>
+      <c r="D202">
+        <v>1.1006338777425</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <v>0.932226226727773</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>813</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished all data preproccessing before thresholding
</commit_message>
<xml_diff>
--- a/data/Mass Spec and Protein Properties 200CMNP.xlsx
+++ b/data/Mass Spec and Protein Properties 200CMNP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavo/PycharmProjects/swnt-protein-corona-ML/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340340EF-5F56-4945-8A43-5A3B1F9D0D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393D96E8-6FE0-B74B-8701-F84D28446B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="822">
   <si>
     <t>Entry</t>
   </si>
@@ -2477,13 +2477,16 @@
     <t>Accession</t>
   </si>
   <si>
-    <t>Relative Abundance_1</t>
-  </si>
-  <si>
-    <t>Relative Abundance_2</t>
-  </si>
-  <si>
-    <t>Relative Abundance_3</t>
+    <t>NP Relative Abundance_1</t>
+  </si>
+  <si>
+    <t>NP Relative Abundance_2</t>
+  </si>
+  <si>
+    <t>NP Relative Abundance_3</t>
+  </si>
+  <si>
+    <t>FBS Relative Abundance</t>
   </si>
 </sst>
 </file>
@@ -6321,18 +6324,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67499FF8-0E27-8146-BF0C-A25E26B61179}">
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>817</v>
       </c>
@@ -6345,8 +6349,11 @@
       <c r="D1" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6359,8 +6366,11 @@
       <c r="D2">
         <v>1385.3965053289501</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>7936.6759421998204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6373,8 +6383,11 @@
       <c r="D3">
         <v>738.34407099021803</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>73.655740637978397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -6387,8 +6400,11 @@
       <c r="D4">
         <v>682.86473093507595</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>16.734757072340201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -6401,8 +6417,11 @@
       <c r="D5">
         <v>750.86842591587595</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>32.812876456881398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -6415,8 +6434,11 @@
       <c r="D6">
         <v>1133.39567822666</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>4017.7153557566198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -6429,8 +6451,11 @@
       <c r="D7">
         <v>934.93984133782203</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>25.490070242486301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6443,8 +6468,11 @@
       <c r="D8">
         <v>893.49775942747704</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>145.88588629586599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -6457,8 +6485,11 @@
       <c r="D9">
         <v>734.02871915415005</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>101.675161973927</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -6471,8 +6502,11 @@
       <c r="D10">
         <v>917.80249345429797</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>2688.3265613144099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -6485,8 +6519,11 @@
       <c r="D11">
         <v>699.48127034545405</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>3.8541608284448698</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -6499,8 +6536,11 @@
       <c r="D12">
         <v>694.57069975578997</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>26.5601304745113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -6513,8 +6553,11 @@
       <c r="D13">
         <v>502.53824144075298</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>18.400975205130099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -6527,8 +6570,11 @@
       <c r="D14">
         <v>628.10460560427896</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>17.3317789700627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -6541,8 +6587,11 @@
       <c r="D15">
         <v>419.75321725566198</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>6.6717845068207504</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -6555,8 +6604,11 @@
       <c r="D16">
         <v>429.74794009603801</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>83.997784220812406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -6569,8 +6621,11 @@
       <c r="D17">
         <v>410.94893192247599</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>21.516116235865901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -6583,8 +6638,11 @@
       <c r="D18">
         <v>430.83917447763002</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>7.6329811221844004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -6597,8 +6655,11 @@
       <c r="D19">
         <v>372.80534600205698</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>68.337839363764203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -6611,8 +6672,11 @@
       <c r="D20">
         <v>336.74499397422198</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>58.198835065973299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -6625,8 +6689,11 @@
       <c r="D21">
         <v>364.69548254806699</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>32.941612003568302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -6639,8 +6706,11 @@
       <c r="D22">
         <v>304.03278711661301</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -6653,8 +6723,11 @@
       <c r="D23">
         <v>270.00611503606302</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -6667,8 +6740,11 @@
       <c r="D24">
         <v>289.127493686572</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>252.01063260158901</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -6681,8 +6757,11 @@
       <c r="D25">
         <v>240.28236662400701</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>61.710982698740203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -6695,8 +6774,11 @@
       <c r="D26">
         <v>213.636407088043</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>46.301596959404797</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -6709,8 +6791,11 @@
       <c r="D27">
         <v>218.58664305544599</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -6723,8 +6808,11 @@
       <c r="D28">
         <v>228.24655137880001</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>113</v>
       </c>
@@ -6737,8 +6825,11 @@
       <c r="D29">
         <v>199.76533401924999</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -6751,8 +6842,11 @@
       <c r="D30">
         <v>183.75642565754299</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -6765,8 +6859,11 @@
       <c r="D31">
         <v>177.95304280998499</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -6779,8 +6876,11 @@
       <c r="D32">
         <v>183.90275423592701</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>36.931549953904799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -6793,8 +6893,11 @@
       <c r="D33">
         <v>154.749431732316</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -6807,8 +6910,11 @@
       <c r="D34">
         <v>148.199549332749</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -6821,8 +6927,11 @@
       <c r="D35">
         <v>132.08400157914801</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -6835,8 +6944,11 @@
       <c r="D36">
         <v>124.601601862698</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -6849,8 +6961,11 @@
       <c r="D37">
         <v>135.662750367016</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -6863,8 +6978,11 @@
       <c r="D38">
         <v>107.727150198262</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -6877,8 +6995,11 @@
       <c r="D39">
         <v>116.732317892661</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>42.6529378073323</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -6891,8 +7012,11 @@
       <c r="D40">
         <v>100.26212293316701</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>161</v>
       </c>
@@ -6905,8 +7029,11 @@
       <c r="D41">
         <v>108.49349831164101</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>165</v>
       </c>
@@ -6919,8 +7046,11 @@
       <c r="D42">
         <v>109.542567396729</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -6933,8 +7063,11 @@
       <c r="D43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>173</v>
       </c>
@@ -6947,8 +7080,11 @@
       <c r="D44">
         <v>114.81769756859499</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>78.066445106680803</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>177</v>
       </c>
@@ -6961,8 +7097,11 @@
       <c r="D45">
         <v>105.274356885945</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>181</v>
       </c>
@@ -6975,8 +7114,11 @@
       <c r="D46">
         <v>98.057329498598605</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>1.3808831375325299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>185</v>
       </c>
@@ -6989,8 +7131,11 @@
       <c r="D47">
         <v>83.107418470788602</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>189</v>
       </c>
@@ -7003,8 +7148,11 @@
       <c r="D48">
         <v>90.341810373240406</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>30.337525173270699</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>193</v>
       </c>
@@ -7017,8 +7165,11 @@
       <c r="D49">
         <v>71.9495508871357</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>7.92674008777868</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>197</v>
       </c>
@@ -7031,8 +7182,11 @@
       <c r="D50">
         <v>82.909012219589997</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>324.21053145398503</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -7045,8 +7199,11 @@
       <c r="D51">
         <v>78.549034849502107</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>205</v>
       </c>
@@ -7059,8 +7216,11 @@
       <c r="D52">
         <v>75.828393098067195</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>1125.7016084485399</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>209</v>
       </c>
@@ -7073,8 +7233,11 @@
       <c r="D53">
         <v>57.937105428113703</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>213</v>
       </c>
@@ -7087,8 +7250,11 @@
       <c r="D54">
         <v>64.008336714789095</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>217</v>
       </c>
@@ -7101,8 +7267,11 @@
       <c r="D55">
         <v>53.145594461668999</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>6.88691974927068</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -7115,8 +7284,11 @@
       <c r="D56">
         <v>61.887869905104701</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>69.257996123640396</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>225</v>
       </c>
@@ -7129,8 +7301,11 @@
       <c r="D57">
         <v>62.964223817856798</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>485.09107803754898</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>229</v>
       </c>
@@ -7143,8 +7318,11 @@
       <c r="D58">
         <v>59.8542058303196</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>233</v>
       </c>
@@ -7157,8 +7335,11 @@
       <c r="D59">
         <v>63.529681633772597</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>404.22530352407398</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>237</v>
       </c>
@@ -7171,8 +7352,11 @@
       <c r="D60">
         <v>57.396448393597701</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>175.57282176004199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>241</v>
       </c>
@@ -7185,8 +7369,11 @@
       <c r="D61">
         <v>53.440723760326797</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>520.86055208344101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>245</v>
       </c>
@@ -7199,8 +7386,11 @@
       <c r="D62">
         <v>53.406002666367101</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>9.3259831606608596</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>249</v>
       </c>
@@ -7213,8 +7403,11 @@
       <c r="D63">
         <v>51.362418279022101</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>253</v>
       </c>
@@ -7227,8 +7420,11 @@
       <c r="D64">
         <v>46.697391297716401</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>257</v>
       </c>
@@ -7241,8 +7437,11 @@
       <c r="D65">
         <v>42.275411974129</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>261</v>
       </c>
@@ -7255,8 +7454,11 @@
       <c r="D66">
         <v>41.3106615776761</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>15.249114303695</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>265</v>
       </c>
@@ -7269,8 +7471,11 @@
       <c r="D67">
         <v>42.449017443927701</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>269</v>
       </c>
@@ -7283,8 +7488,11 @@
       <c r="D68">
         <v>40.422793603562603</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>4.0321010018688197</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>273</v>
       </c>
@@ -7297,8 +7505,11 @@
       <c r="D69">
         <v>40.040861570005397</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>277</v>
       </c>
@@ -7311,8 +7522,11 @@
       <c r="D70">
         <v>36.506750220531401</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>281</v>
       </c>
@@ -7325,8 +7539,11 @@
       <c r="D71">
         <v>36.821720144309097</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>285</v>
       </c>
@@ -7339,8 +7556,11 @@
       <c r="D72">
         <v>36.246342015833299</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>289</v>
       </c>
@@ -7353,8 +7573,11 @@
       <c r="D73">
         <v>32.057490037404101</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>76.100852028071998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>293</v>
       </c>
@@ -7367,8 +7590,11 @@
       <c r="D74">
         <v>35.266711150540502</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>75.884852788664404</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>297</v>
       </c>
@@ -7381,8 +7607,11 @@
       <c r="D75">
         <v>36.784518972209398</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>301</v>
       </c>
@@ -7395,8 +7624,11 @@
       <c r="D76">
         <v>33.629859578152598</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>20.8607745435034</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>305</v>
       </c>
@@ -7409,8 +7641,11 @@
       <c r="D77">
         <v>30.442959168276001</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>309</v>
       </c>
@@ -7423,8 +7658,11 @@
       <c r="D78">
         <v>28.0695243883135</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>313</v>
       </c>
@@ -7437,8 +7675,11 @@
       <c r="D79">
         <v>25.3141575747937</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>317</v>
       </c>
@@ -7451,8 +7692,11 @@
       <c r="D80">
         <v>27.962881028294198</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>178.454244701763</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>321</v>
       </c>
@@ -7465,8 +7709,11 @@
       <c r="D81">
         <v>20.902098563766199</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>325</v>
       </c>
@@ -7479,8 +7726,11 @@
       <c r="D82">
         <v>20.861425282270499</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>329</v>
       </c>
@@ -7493,8 +7743,11 @@
       <c r="D83">
         <v>22.884425021053602</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <v>7.5824373001630301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>333</v>
       </c>
@@ -7507,8 +7760,11 @@
       <c r="D84">
         <v>26.566597035484499</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>337</v>
       </c>
@@ -7521,8 +7777,11 @@
       <c r="D85">
         <v>24.1011513565287</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>341</v>
       </c>
@@ -7535,8 +7794,11 @@
       <c r="D86">
         <v>21.6939875138624</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>345</v>
       </c>
@@ -7549,8 +7811,11 @@
       <c r="D87">
         <v>20.401866802931899</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>349</v>
       </c>
@@ -7563,8 +7828,11 @@
       <c r="D88">
         <v>21.021638330113301</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>353</v>
       </c>
@@ -7577,8 +7845,11 @@
       <c r="D89">
         <v>19.5933613292978</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>357</v>
       </c>
@@ -7591,8 +7862,11 @@
       <c r="D90">
         <v>18.6541557376867</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>361</v>
       </c>
@@ -7605,8 +7879,11 @@
       <c r="D91">
         <v>20.2237971924812</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <v>359.53072708191002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>365</v>
       </c>
@@ -7619,8 +7896,11 @@
       <c r="D92">
         <v>20.304151724216599</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>369</v>
       </c>
@@ -7633,8 +7913,11 @@
       <c r="D93">
         <v>17.940389248999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <v>11.0155292113068</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>373</v>
       </c>
@@ -7647,8 +7930,11 @@
       <c r="D94">
         <v>20.099545277668099</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <v>147.782352705889</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>377</v>
       </c>
@@ -7661,8 +7947,11 @@
       <c r="D95">
         <v>16.337514747129799</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>381</v>
       </c>
@@ -7675,8 +7964,11 @@
       <c r="D96">
         <v>17.4649582695655</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>385</v>
       </c>
@@ -7689,8 +7981,11 @@
       <c r="D97">
         <v>17.657164325414101</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>389</v>
       </c>
@@ -7703,8 +7998,11 @@
       <c r="D98">
         <v>16.875195687877799</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>4.5847998556648903</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>393</v>
       </c>
@@ -7717,8 +8015,11 @@
       <c r="D99">
         <v>16.022544823352099</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>397</v>
       </c>
@@ -7731,8 +8032,11 @@
       <c r="D100">
         <v>16.258152246650301</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>401</v>
       </c>
@@ -7745,8 +8049,11 @@
       <c r="D101">
         <v>14.3008745785767</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>405</v>
       </c>
@@ -7759,8 +8066,11 @@
       <c r="D102">
         <v>15.2591767718657</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>409</v>
       </c>
@@ -7773,8 +8083,11 @@
       <c r="D103">
         <v>14.7465446203315</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>413</v>
       </c>
@@ -7787,8 +8100,11 @@
       <c r="D104">
         <v>13.253785587876401</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <v>39.426341169062098</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>417</v>
       </c>
@@ -7801,8 +8117,11 @@
       <c r="D105">
         <v>7.1587455510573301</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <v>19.833050162402198</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>421</v>
       </c>
@@ -7815,8 +8134,11 @@
       <c r="D106">
         <v>13.6062046915679</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>425</v>
       </c>
@@ -7829,8 +8151,11 @@
       <c r="D107">
         <v>10.221642053934801</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>429</v>
       </c>
@@ -7843,8 +8168,11 @@
       <c r="D108">
         <v>10.466673774165001</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>433</v>
       </c>
@@ -7857,8 +8185,11 @@
       <c r="D109">
         <v>11.8743661264186</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>437</v>
       </c>
@@ -7871,8 +8202,11 @@
       <c r="D110">
         <v>7.9942838764171897</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>441</v>
       </c>
@@ -7885,8 +8219,11 @@
       <c r="D111">
         <v>10.740970416446901</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>445</v>
       </c>
@@ -7899,8 +8236,11 @@
       <c r="D112">
         <v>10.5336358839445</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>449</v>
       </c>
@@ -7913,8 +8253,11 @@
       <c r="D113">
         <v>11.5936212809727</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>453</v>
       </c>
@@ -7927,8 +8270,11 @@
       <c r="D114">
         <v>11.0685887387385</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>457</v>
       </c>
@@ -7941,8 +8287,11 @@
       <c r="D115">
         <v>10.327045374883999</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>461</v>
       </c>
@@ -7955,8 +8304,11 @@
       <c r="D116">
         <v>9.7576194339442193</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>465</v>
       </c>
@@ -7969,8 +8321,11 @@
       <c r="D117">
         <v>8.9568022025441092</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>469</v>
       </c>
@@ -7983,8 +8338,11 @@
       <c r="D118">
         <v>8.2980934485649502</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>473</v>
       </c>
@@ -7997,8 +8355,11 @@
       <c r="D119">
         <v>9.7968046685559198</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <v>17.5352502535846</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>477</v>
       </c>
@@ -8011,8 +8372,11 @@
       <c r="D120">
         <v>9.7625795902241794</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <v>96.797899148104506</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>481</v>
       </c>
@@ -8025,8 +8389,11 @@
       <c r="D121">
         <v>9.3856077129469497</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>485</v>
       </c>
@@ -8039,8 +8406,11 @@
       <c r="D122">
         <v>8.6750653258421799</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E122">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>489</v>
       </c>
@@ -8053,8 +8423,11 @@
       <c r="D123">
         <v>9.93072888811494</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>493</v>
       </c>
@@ -8067,8 +8440,11 @@
       <c r="D124">
         <v>9.4902670104541809</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E124">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>497</v>
       </c>
@@ -8081,8 +8457,11 @@
       <c r="D125">
         <v>7.9245936806837003</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E125">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>501</v>
       </c>
@@ -8095,8 +8474,11 @@
       <c r="D126">
         <v>9.5986464251713794</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E126">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>505</v>
       </c>
@@ -8109,8 +8491,11 @@
       <c r="D127">
         <v>8.9734187260819809</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E127">
+        <v>31.8655037928398</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>509</v>
       </c>
@@ -8123,8 +8508,11 @@
       <c r="D128">
         <v>9.1438000942987294</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E128">
+        <v>19.274908127773099</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>513</v>
       </c>
@@ -8137,8 +8525,11 @@
       <c r="D129">
         <v>7.9231056337997101</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E129">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>517</v>
       </c>
@@ -8151,8 +8542,11 @@
       <c r="D130">
         <v>7.5627502800603601</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>521</v>
       </c>
@@ -8165,8 +8559,11 @@
       <c r="D131">
         <v>8.3290944253147199</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E131">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>525</v>
       </c>
@@ -8179,8 +8576,11 @@
       <c r="D132">
         <v>8.7073063416619405</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>529</v>
       </c>
@@ -8193,8 +8593,11 @@
       <c r="D133">
         <v>9.27450021227577</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E133">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>533</v>
       </c>
@@ -8207,8 +8610,11 @@
       <c r="D134">
         <v>6.9675315264647404</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E134">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>537</v>
       </c>
@@ -8221,8 +8627,11 @@
       <c r="D135">
         <v>7.8586236021601801</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E135">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>541</v>
       </c>
@@ -8235,8 +8644,11 @@
       <c r="D136">
         <v>8.1773136431478406</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E136">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>545</v>
       </c>
@@ -8249,8 +8661,11 @@
       <c r="D137">
         <v>6.8842009009613498</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E137">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>549</v>
       </c>
@@ -8263,8 +8678,11 @@
       <c r="D138">
         <v>7.1096400038856897</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E138">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>553</v>
       </c>
@@ -8277,8 +8695,11 @@
       <c r="D139">
         <v>6.5724550787656497</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E139">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>557</v>
       </c>
@@ -8291,8 +8712,11 @@
       <c r="D140">
         <v>7.5999514521600897</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E140">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>561</v>
       </c>
@@ -8305,8 +8729,11 @@
       <c r="D141">
         <v>6.0565988256494396</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E141">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>565</v>
       </c>
@@ -8319,8 +8746,11 @@
       <c r="D142">
         <v>6.5305417581999503</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E142">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>569</v>
       </c>
@@ -8333,8 +8763,11 @@
       <c r="D143">
         <v>8.9833390386419101</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E143">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>573</v>
       </c>
@@ -8347,8 +8780,11 @@
       <c r="D144">
         <v>5.8527364025429396</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E144">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>577</v>
       </c>
@@ -8361,8 +8797,11 @@
       <c r="D145">
         <v>9.9684260758426593</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E145">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>581</v>
       </c>
@@ -8375,8 +8814,11 @@
       <c r="D146">
         <v>6.1835788264165101</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E146">
+        <v>5.9874989163775902</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>585</v>
       </c>
@@ -8389,8 +8831,11 @@
       <c r="D147">
         <v>7.1934666450170797</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E147">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>589</v>
       </c>
@@ -8403,8 +8848,11 @@
       <c r="D148">
         <v>6.0332860911336104</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E148">
+        <v>50.569741930098203</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>593</v>
       </c>
@@ -8417,8 +8865,11 @@
       <c r="D149">
         <v>4.9626363581034898</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E149">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>597</v>
       </c>
@@ -8431,8 +8882,11 @@
       <c r="D150">
         <v>3.9351399847090498</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E150">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>601</v>
       </c>
@@ -8445,8 +8899,11 @@
       <c r="D151">
         <v>7.3539277006738999</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E151">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>605</v>
       </c>
@@ -8459,8 +8916,11 @@
       <c r="D152">
         <v>4.5387910039806103</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E152">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>609</v>
       </c>
@@ -8473,8 +8933,11 @@
       <c r="D153">
         <v>6.4159621481327997</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E153">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>613</v>
       </c>
@@ -8487,8 +8950,11 @@
       <c r="D154">
         <v>7.1322087149595301</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E154">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>617</v>
       </c>
@@ -8501,8 +8967,11 @@
       <c r="D155">
         <v>4.7009881143354102</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E155">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>621</v>
       </c>
@@ -8515,8 +8984,11 @@
       <c r="D156">
         <v>6.0526307006254703</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E156">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>625</v>
       </c>
@@ -8529,8 +9001,11 @@
       <c r="D157">
         <v>5.1903075313538096</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E157">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>629</v>
       </c>
@@ -8543,8 +9018,11 @@
       <c r="D158">
         <v>4.6875956923795101</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E158">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>633</v>
       </c>
@@ -8557,8 +9035,11 @@
       <c r="D159">
         <v>3.59313720920556</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E159">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>637</v>
       </c>
@@ -8571,8 +9052,11 @@
       <c r="D160">
         <v>4.7934950289567304</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E160">
+        <v>29.349544652220601</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>641</v>
       </c>
@@ -8585,8 +9069,11 @@
       <c r="D161">
         <v>5.3150554617948904</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E161">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>645</v>
       </c>
@@ -8599,8 +9086,11 @@
       <c r="D162">
         <v>4.75182971620504</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E162">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>649</v>
       </c>
@@ -8613,8 +9103,11 @@
       <c r="D163">
         <v>4.4807571755050297</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E163">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>653</v>
       </c>
@@ -8627,8 +9120,11 @@
       <c r="D164">
         <v>5.0452229601648799</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E164">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>657</v>
       </c>
@@ -8641,8 +9137,11 @@
       <c r="D165">
         <v>5.0221582334630499</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E165">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>661</v>
       </c>
@@ -8655,8 +9154,11 @@
       <c r="D166">
         <v>4.2203489708069499</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E166">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>665</v>
       </c>
@@ -8669,8 +9171,11 @@
       <c r="D167">
         <v>3.8294886559458199</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E167">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>669</v>
       </c>
@@ -8683,8 +9188,11 @@
       <c r="D168">
         <v>4.6454343639998203</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E168">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>673</v>
       </c>
@@ -8697,8 +9205,11 @@
       <c r="D169">
         <v>3.0291674401737101</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E169">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>677</v>
       </c>
@@ -8711,8 +9222,11 @@
       <c r="D170">
         <v>5.34630444635867</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E170">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>681</v>
       </c>
@@ -8725,8 +9239,11 @@
       <c r="D171">
         <v>5.2056840158217002</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E171">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>685</v>
       </c>
@@ -8739,8 +9256,11 @@
       <c r="D172">
         <v>4.5363109258406196</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E172">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>689</v>
       </c>
@@ -8753,8 +9273,11 @@
       <c r="D173">
         <v>3.6819240066169101</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E173">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>693</v>
       </c>
@@ -8767,8 +9290,11 @@
       <c r="D174">
         <v>3.1010897062331799</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E174">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>697</v>
       </c>
@@ -8781,8 +9307,11 @@
       <c r="D175">
         <v>3.3766263875851599</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E175">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>701</v>
       </c>
@@ -8795,8 +9324,11 @@
       <c r="D176">
         <v>3.22806970700025</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E176">
+        <v>5.9080111962756101</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>705</v>
       </c>
@@ -8809,8 +9341,11 @@
       <c r="D177">
         <v>4.3877542452557199</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E177">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>709</v>
       </c>
@@ -8823,8 +9358,11 @@
       <c r="D178">
         <v>3.9825094771826999</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E178">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>713</v>
       </c>
@@ -8837,8 +9375,11 @@
       <c r="D179">
         <v>4.6360100670678897</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E179">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>717</v>
       </c>
@@ -8851,8 +9392,11 @@
       <c r="D180">
         <v>3.3657140437692399</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E180">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>721</v>
       </c>
@@ -8865,8 +9409,11 @@
       <c r="D181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E181">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>725</v>
       </c>
@@ -8879,8 +9426,11 @@
       <c r="D182">
         <v>3.8027038120340202</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E182">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>729</v>
       </c>
@@ -8893,8 +9443,11 @@
       <c r="D183">
         <v>5.9110182388325097</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E183">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>733</v>
       </c>
@@ -8907,8 +9460,11 @@
       <c r="D184">
         <v>5.3465524541726603</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E184">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>737</v>
       </c>
@@ -8921,8 +9477,11 @@
       <c r="D185">
         <v>2.3227667835627099</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E185">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>741</v>
       </c>
@@ -8935,8 +9494,11 @@
       <c r="D186">
         <v>2.7355261883998701</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E186">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>745</v>
       </c>
@@ -8949,8 +9511,11 @@
       <c r="D187">
         <v>3.3734022860031798</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E187">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>749</v>
       </c>
@@ -8963,8 +9528,11 @@
       <c r="D188">
         <v>2.5353838825033401</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E188">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>753</v>
       </c>
@@ -8977,8 +9545,11 @@
       <c r="D189">
         <v>3.5274151384960502</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E189">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>757</v>
       </c>
@@ -8991,8 +9562,11 @@
       <c r="D190">
         <v>1.8841649645069301</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E190">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>761</v>
       </c>
@@ -9005,8 +9579,11 @@
       <c r="D191">
         <v>3.2766792385438901</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E191">
+        <v>6.0419307247083003</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>765</v>
       </c>
@@ -9019,8 +9596,11 @@
       <c r="D192">
         <v>2.0817775907006801</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E192">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>769</v>
       </c>
@@ -9033,8 +9613,11 @@
       <c r="D193">
         <v>1.2503561950532001</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E193">
+        <v>7.3297181900561803</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>773</v>
       </c>
@@ -9047,8 +9630,11 @@
       <c r="D194">
         <v>2.6636039223404002</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E194">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>777</v>
       </c>
@@ -9061,8 +9647,11 @@
       <c r="D195">
         <v>4.1595870563773998</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E195">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>781</v>
       </c>
@@ -9075,8 +9664,11 @@
       <c r="D196">
         <v>1.6771280413812599</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E196">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>785</v>
       </c>
@@ -9089,8 +9681,11 @@
       <c r="D197">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E197">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>789</v>
       </c>
@@ -9103,8 +9698,11 @@
       <c r="D198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E198">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>793</v>
       </c>
@@ -9117,8 +9715,11 @@
       <c r="D199">
         <v>2.6030900157248502</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E199">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>797</v>
       </c>
@@ -9131,8 +9732,11 @@
       <c r="D200">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E200">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>801</v>
       </c>
@@ -9145,8 +9749,11 @@
       <c r="D201">
         <v>1.9458693086296801</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E201">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>805</v>
       </c>
@@ -9159,8 +9766,11 @@
       <c r="D202">
         <v>1.1006338777425</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E202">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>809</v>
       </c>
@@ -9173,8 +9783,11 @@
       <c r="D203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E203">
+        <v>4.3199847881512203E-2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>813</v>
       </c>
@@ -9186,6 +9799,9 @@
       </c>
       <c r="D204">
         <v>0</v>
+      </c>
+      <c r="E204">
+        <v>4.3199847881512203E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>